<commit_message>
Reconnect Nets after length tuning
</commit_message>
<xml_diff>
--- a/DRAM_Length_Tuning.xlsx
+++ b/DRAM_Length_Tuning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hansg\Documents\SimpleSBC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E014DA1E-BAAA-40BE-B892-EB402736F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F0DA3E-8C82-4EAE-9BEE-BC154F704AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{7BF8155A-85EB-4431-A128-00DAB0CEDDCE}"/>
+    <workbookView xWindow="7200" yWindow="-120" windowWidth="21600" windowHeight="11295" xr2:uid="{7BF8155A-85EB-4431-A128-00DAB0CEDDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902D2B27-2BDF-41BE-8FEC-CA1185437E7F}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -718,7 +720,7 @@
         <v>36</v>
       </c>
       <c r="B22">
-        <v>28.88</v>
+        <v>28.91</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -726,7 +728,7 @@
         <v>37</v>
       </c>
       <c r="B23">
-        <v>29</v>
+        <v>28.91</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>